<commit_message>
Added headings to my figures
</commit_message>
<xml_diff>
--- a/Submissions/HW1_BoxModel_Hsieh.xlsx
+++ b/Submissions/HW1_BoxModel_Hsieh.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnahh\Desktop\GW_Modeling\homework-hsiehdf\Working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnahh\Desktop\GW_Modeling\homework-hsiehdf\Submissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB908409-55A5-45A3-9999-0585D69F0BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCF6CBF-4D20-464A-924F-81353E736CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="2" r:id="rId1"/>
@@ -518,37 +518,37 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91.664648883557263</c:v>
+                  <c:v>99.790740143207117</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>83.329568098852761</c:v>
+                  <c:v>99.581539204987394</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74.994856594139677</c:v>
+                  <c:v>99.372413981615907</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>66.660581952310991</c:v>
+                  <c:v>96.654048430365066</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>58.326777964792377</c:v>
+                  <c:v>91.426976587783699</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>49.993444631552634</c:v>
+                  <c:v>86.200659489716102</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41.660550424709882</c:v>
+                  <c:v>80.975194528297166</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33.32803651246757</c:v>
+                  <c:v>75.750576577625736</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24.99582252911302</c:v>
+                  <c:v>62.68977582828429</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16.663813400996126</c:v>
+                  <c:v>41.79301157147664</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.3319067004980631</c:v>
+                  <c:v>20.896505785738317</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -882,40 +882,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="1">
-                  <c:v>1.6670702232885474E-4</c:v>
+                  <c:v>4.1851971358576633E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6670161569409003E-4</c:v>
+                  <c:v>4.1840187643944662E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6669423009426168E-4</c:v>
+                  <c:v>4.1825044674297373E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6668549283657371E-4</c:v>
+                  <c:v>4.1821008480782165E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6667607975037228E-4</c:v>
+                  <c:v>4.1816574740650931E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6666666666479487E-4</c:v>
+                  <c:v>4.1810536784540772E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6665788413685505E-4</c:v>
+                  <c:v>4.1803719691351491E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6665027824484623E-4</c:v>
+                  <c:v>4.1796943605371437E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.66644279667091E-4</c:v>
+                  <c:v>4.1794562397892628E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.6664018256233788E-4</c:v>
+                  <c:v>4.1793528513615305E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.6663813400996126E-4</c:v>
+                  <c:v>4.1793011571476644E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.6663813400996126E-4</c:v>
+                  <c:v>4.1793011571476633E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2014,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="D7" s="7">
         <f>SUM(L9:L19)+0.5*(L8+L20)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -2120,18 +2120,18 @@
       </c>
       <c r="D8" s="7">
         <f>SUM(M9:M19)+0.5*(M8+M20)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="F8" s="1">
         <f>F9+inputs!$D$8</f>
         <v>60</v>
       </c>
       <c r="G8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H8" s="1">
         <f>IF(G8=1,+inputs!$D$11,+IF(G8=2,+inputs!$D$12,+inputs!$D$13))</f>
-        <v>1E-4</v>
+        <v>0.01</v>
       </c>
       <c r="I8" s="2">
         <f>inputs!D4</f>
@@ -2144,11 +2144,11 @@
       </c>
       <c r="M8">
         <f>IF($G8=2,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8">
         <f>IF($G8=3,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="16">
         <v>1</v>
@@ -2170,26 +2170,26 @@
       </c>
       <c r="D9" s="7">
         <f>SUM(N9:N19)+0.5*(N8+N20)</f>
-        <v>12</v>
+        <v>3.5</v>
       </c>
       <c r="F9" s="1">
         <f>F10+inputs!$D$8</f>
         <v>55</v>
       </c>
       <c r="G9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H9" s="1">
         <f>IF(G9=1,+inputs!$D$11,+IF(G9=2,+inputs!$D$12,+inputs!$D$13))</f>
-        <v>1E-4</v>
+        <v>0.01</v>
       </c>
       <c r="I9" s="1">
         <f ca="1">(I8*2/(1/H8+1/H9)+I10*2/(1/H9+1/H10))/(2/(1/H8+1/H9)+2/(1/H9+1/H10))</f>
-        <v>91.664648883557263</v>
+        <v>99.790740143207117</v>
       </c>
       <c r="J9" s="1">
         <f ca="1">(I8-I9)/inputs!$D$8*2/(1/H8+1/H9)</f>
-        <v>1.6670702232885474E-4</v>
+        <v>4.1851971358576633E-4</v>
       </c>
       <c r="L9">
         <f t="shared" ref="L9:L20" si="0">IF($G9=1,1,0)</f>
@@ -2197,11 +2197,11 @@
       </c>
       <c r="M9">
         <f t="shared" ref="M9:M20" si="1">IF($G9=2,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9">
         <f t="shared" ref="N9:N20" si="2">IF($G9=3,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="16">
         <v>2</v>
@@ -2223,19 +2223,19 @@
         <v>50</v>
       </c>
       <c r="G10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H10" s="1">
         <f>IF(G10=1,+inputs!$D$11,+IF(G10=2,+inputs!$D$12,+inputs!$D$13))</f>
-        <v>1E-4</v>
+        <v>0.01</v>
       </c>
       <c r="I10" s="1">
         <f ca="1">(I9*2/(1/H9+1/H10)+I11*2/(1/H10+1/H11))/(2/(1/H9+1/H10)+2/(1/H10+1/H11))</f>
-        <v>83.329568098852761</v>
+        <v>99.581539204987394</v>
       </c>
       <c r="J10" s="1">
         <f ca="1">(I9-I10)/inputs!$D$8*2/(1/H9+1/H10)</f>
-        <v>1.6670161569409003E-4</v>
+        <v>4.1840187643944662E-4</v>
       </c>
       <c r="L10">
         <f t="shared" si="0"/>
@@ -2243,11 +2243,11 @@
       </c>
       <c r="M10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="16">
         <v>3</v>
@@ -2266,7 +2266,7 @@
       </c>
       <c r="C11" s="6">
         <f>SUM(D7:D9)/(D7/C7+D8/C8+D9/C9)</f>
-        <v>1E-4</v>
+        <v>2.5078369905956113E-4</v>
       </c>
       <c r="D11" s="7"/>
       <c r="F11" s="1">
@@ -2274,19 +2274,19 @@
         <v>45</v>
       </c>
       <c r="G11" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H11" s="1">
         <f>IF(G11=1,+inputs!$D$11,+IF(G11=2,+inputs!$D$12,+inputs!$D$13))</f>
-        <v>1E-4</v>
+        <v>0.01</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" ref="I11:I19" ca="1" si="3">(I10*2/(1/H10+1/H11)+I12*2/(1/H11+1/H12))/(2/(1/H10+1/H11)+2/(1/H11+1/H12))</f>
-        <v>74.994856594139677</v>
+        <v>99.372413981615907</v>
       </c>
       <c r="J11" s="1">
         <f ca="1">(I10-I11)/inputs!$D$8*2/(1/H10+1/H11)</f>
-        <v>1.6669423009426168E-4</v>
+        <v>4.1825044674297373E-4</v>
       </c>
       <c r="L11">
         <f>IF($G11=1,1,0)</f>
@@ -2294,11 +2294,11 @@
       </c>
       <c r="M11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="16">
         <v>4</v>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="C12" s="9">
         <f>C11*(I8-I20)/(F8-F20)</f>
-        <v>1.6666666666666666E-4</v>
+        <v>4.1797283176593522E-4</v>
       </c>
       <c r="D12" s="10"/>
       <c r="F12" s="1">
@@ -2325,23 +2325,23 @@
         <v>40</v>
       </c>
       <c r="G12" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H12" s="1">
         <f>IF(G12=1,+inputs!$D$11,+IF(G12=2,+inputs!$D$12,+inputs!$D$13))</f>
-        <v>1E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>66.660581952310991</v>
+        <v>96.654048430365066</v>
       </c>
       <c r="J12" s="1">
         <f ca="1">(I11-I12)/inputs!$D$8*2/(1/H11+1/H12)</f>
-        <v>1.6668549283657371E-4</v>
+        <v>4.1821008480782165E-4</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12">
         <f t="shared" si="1"/>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="N12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="16">
         <v>5</v>
@@ -2368,23 +2368,23 @@
         <v>35</v>
       </c>
       <c r="G13" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H13" s="1">
         <f>IF(G13=1,+inputs!$D$11,+IF(G13=2,+inputs!$D$12,+inputs!$D$13))</f>
-        <v>1E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>58.326777964792377</v>
+        <v>91.426976587783699</v>
       </c>
       <c r="J13" s="1">
         <f ca="1">(I12-I13)/inputs!$D$8*2/(1/H12+1/H13)</f>
-        <v>1.6667607975037228E-4</v>
+        <v>4.1816574740650931E-4</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13">
         <f t="shared" si="1"/>
@@ -2392,7 +2392,7 @@
       </c>
       <c r="N13">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="16">
         <v>6</v>
@@ -2411,23 +2411,23 @@
         <v>30</v>
       </c>
       <c r="G14" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1">
         <f>IF(G14=1,+inputs!$D$11,+IF(G14=2,+inputs!$D$12,+inputs!$D$13))</f>
-        <v>1E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>49.993444631552634</v>
+        <v>86.200659489716102</v>
       </c>
       <c r="J14" s="1">
         <f ca="1">(I13-I14)/inputs!$D$8*2/(1/H13+1/H14)</f>
-        <v>1.6666666666479487E-4</v>
+        <v>4.1810536784540772E-4</v>
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14">
         <f t="shared" si="1"/>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="16">
         <v>7</v>
@@ -2454,23 +2454,23 @@
         <v>25</v>
       </c>
       <c r="G15" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H15" s="1">
         <f>IF(G15=1,+inputs!$D$11,+IF(G15=2,+inputs!$D$12,+inputs!$D$13))</f>
-        <v>1E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>41.660550424709882</v>
+        <v>80.975194528297166</v>
       </c>
       <c r="J15" s="1">
         <f ca="1">(I14-I15)/inputs!$D$8*2/(1/H14+1/H15)</f>
-        <v>1.6665788413685505E-4</v>
+        <v>4.1803719691351491E-4</v>
       </c>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15">
         <f t="shared" si="1"/>
@@ -2478,7 +2478,7 @@
       </c>
       <c r="N15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="16">
         <v>8</v>
@@ -2497,23 +2497,23 @@
         <v>20</v>
       </c>
       <c r="G16" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H16" s="1">
         <f>IF(G16=1,+inputs!$D$11,+IF(G16=2,+inputs!$D$12,+inputs!$D$13))</f>
-        <v>1E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>33.32803651246757</v>
+        <v>75.750576577625736</v>
       </c>
       <c r="J16" s="1">
         <f ca="1">(I15-I16)/inputs!$D$8*2/(1/H15+1/H16)</f>
-        <v>1.6665027824484623E-4</v>
+        <v>4.1796943605371437E-4</v>
       </c>
       <c r="L16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16">
         <f t="shared" si="1"/>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="N16">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="16">
         <v>9</v>
@@ -2548,11 +2548,11 @@
       </c>
       <c r="I17" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>24.99582252911302</v>
+        <v>62.68977582828429</v>
       </c>
       <c r="J17" s="1">
         <f ca="1">(I16-I17)/inputs!$D$8*2/(1/H16+1/H17)</f>
-        <v>1.66644279667091E-4</v>
+        <v>4.1794562397892628E-4</v>
       </c>
       <c r="L17">
         <f t="shared" si="0"/>
@@ -2591,11 +2591,11 @@
       </c>
       <c r="I18" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>16.663813400996126</v>
+        <v>41.79301157147664</v>
       </c>
       <c r="J18" s="1">
         <f ca="1">(I17-I18)/inputs!$D$8*2/(1/H17+1/H18)</f>
-        <v>1.6664018256233788E-4</v>
+        <v>4.1793528513615305E-4</v>
       </c>
       <c r="L18">
         <f t="shared" si="0"/>
@@ -2634,11 +2634,11 @@
       </c>
       <c r="I19" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>8.3319067004980631</v>
+        <v>20.896505785738317</v>
       </c>
       <c r="J19" s="1">
         <f ca="1">(I18-I19)/inputs!$D$8*2/(1/H18+1/H19)</f>
-        <v>1.6663813400996126E-4</v>
+        <v>4.1793011571476644E-4</v>
       </c>
       <c r="L19">
         <f t="shared" si="0"/>
@@ -2681,7 +2681,7 @@
       </c>
       <c r="J20" s="1">
         <f ca="1">(I19-I20)/inputs!$D$8*2/(1/H19+1/H20)</f>
-        <v>1.6663813400996126E-4</v>
+        <v>4.1793011571476633E-4</v>
       </c>
       <c r="L20">
         <f t="shared" si="0"/>

</xml_diff>